<commit_message>
save current change. result still not correct
</commit_message>
<xml_diff>
--- a/docs/Input Variable List.xlsx
+++ b/docs/Input Variable List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\idep\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65503D95-BBE2-4CCA-9575-EDF1FFEEF991}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26148FD-8B0B-46DC-9613-C8490C5621A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5145" windowWidth="29040" windowHeight="15840" xr2:uid="{6748A816-7F86-4003-89A5-37799D2B9C80}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Variable Name</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>noFDR</t>
+  </si>
+  <si>
+    <t>This should change to number/factors</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -250,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -268,21 +274,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -303,6 +300,23 @@
         <vertAlign val="baseline"/>
         <color theme="1"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -338,13 +352,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -359,13 +366,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4CB72E3-EB3A-4EFD-BF37-3FCC5320666C}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4">
-  <autoFilter ref="A1:D1048576" xr:uid="{8BF75C11-3D8C-4CEE-80A1-95855E29B7E1}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4CB72E3-EB3A-4EFD-BF37-3FCC5320666C}" name="Table1" displayName="Table1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3">
+  <autoFilter ref="A1:E1048576" xr:uid="{8BF75C11-3D8C-4CEE-80A1-95855E29B7E1}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A56E1CDE-5B0E-41EE-80EF-7122212161F9}" name="Variable Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{5F44179F-AA2D-4E4D-9B24-61B81093C50F}" name="Avaiable Values" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{5F44179F-AA2D-4E4D-9B24-61B81093C50F}" name="Avaiable Values" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{FC4F324E-1801-4702-86FA-425754170E78}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{171EFFA7-199E-4F0C-BD60-3F7E0C7A9EEB}" name="Old Variable" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{171EFFA7-199E-4F0C-BD60-3F7E0C7A9EEB}" name="Old Variable" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{0F1CC96A-D350-48B1-8902-66D978692B51}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -668,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EDDCDC3-617A-4A21-9148-837CF3BC2AFC}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +690,7 @@
     <col min="4" max="4" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -695,8 +703,11 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -709,8 +720,11 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -721,7 +735,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -735,7 +749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -746,7 +760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
@@ -760,7 +774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
@@ -771,7 +785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
@@ -779,7 +793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
@@ -787,7 +801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>30</v>
       </c>
@@ -795,7 +809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>31</v>
       </c>
@@ -803,7 +817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -814,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -822,7 +836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
im going to die............
</commit_message>
<xml_diff>
--- a/docs/Input Variable List.xlsx
+++ b/docs/Input Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\idep\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26148FD-8B0B-46DC-9613-C8490C5621A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3930D3-8F35-40CA-99D6-B3A6F0B93536}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5145" windowWidth="29040" windowHeight="15840" xr2:uid="{6748A816-7F86-4003-89A5-37799D2B9C80}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6748A816-7F86-4003-89A5-37799D2B9C80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Variable Name</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>selectOrg</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>select the species of sample</t>
   </si>
 </sst>
 </file>
@@ -676,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EDDCDC3-617A-4A21-9148-837CF3BC2AFC}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,6 +853,20 @@
         <v>35</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>